<commit_message>
revert the authentication back to MSO.
</commit_message>
<xml_diff>
--- a/build_mso.xlsx
+++ b/build_mso.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calange/PycharmProjects/pycharm/ansible_ndo_dcnm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calange/PycharmProjects/ansible_ndo_dcnm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35991BD4-B1CF-4A45-A5DA-82D6850E28BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94630481-863C-AA4B-A2B9-C19BC0CCE382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20220" yWindow="-28800" windowWidth="34120" windowHeight="28800" tabRatio="878" firstSheet="8" activeTab="16" xr2:uid="{A9CD2B9B-B0A4-594B-AA2D-F7681573ED79}"/>
+    <workbookView xWindow="-15700" yWindow="-28300" windowWidth="34120" windowHeight="28300" tabRatio="878" activeTab="1" xr2:uid="{A9CD2B9B-B0A4-594B-AA2D-F7681573ED79}"/>
   </bookViews>
   <sheets>
     <sheet name="build_tasks" sheetId="11" r:id="rId1"/>
@@ -32,7 +32,6 @@
     <sheet name="network_site_dhcp_association" sheetId="48" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="97">
   <si>
     <t>include</t>
   </si>
@@ -361,6 +360,9 @@
   </si>
   <si>
     <t>dhcp_address</t>
+  </si>
+  <si>
+    <t>C1sco12345</t>
   </si>
 </sst>
 </file>
@@ -545,10 +547,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -557,10 +558,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -572,6 +573,167 @@
     <cellStyle name="Normal 4" xfId="5" xr:uid="{43D0B8A7-C5A0-4D58-9BEC-3B91BF456DB2}"/>
   </cellStyles>
   <dxfs count="77">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -595,167 +757,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1635,17 +1636,17 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{6DA18C78-B542-9B40-ABB2-01CD41D5D451}" name="network_site_dhcp_association" displayName="network_site_dhcp_association" ref="A1:G2" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{6DA18C78-B542-9B40-ABB2-01CD41D5D451}" name="network_site_dhcp_association" displayName="network_site_dhcp_association" ref="A1:G2" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:G2" xr:uid="{6DA18C78-B542-9B40-ABB2-01CD41D5D451}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5CB6893E-DF39-3B4E-8E4E-2467B57A7FE3}" name="network_name" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{D1170512-1F44-8045-B049-CC9CBBE451B6}" name="network_template_name" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{5CB6893E-DF39-3B4E-8E4E-2467B57A7FE3}" name="network_name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D1170512-1F44-8045-B049-CC9CBBE451B6}" name="network_template_name" dataDxfId="2">
       <calculatedColumnFormula>IF(ISBLANK(network_site_association16[[#This Row],[network_name]]),"",_xlfn.XLOOKUP(network_site_association16[[#This Row],[network_name]],network[name],network[template_name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3FB15CD7-11C8-6147-8E7E-C38DCB0414E7}" name="network_schema_name" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{3FB15CD7-11C8-6147-8E7E-C38DCB0414E7}" name="network_schema_name" dataDxfId="1">
       <calculatedColumnFormula>IF(ISBLANK(network_site_association16[[#This Row],[network_name]]),"",_xlfn.XLOOKUP(network_site_association16[[#This Row],[network_name]],network[name],network[schema_name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BA067983-0C25-7A45-B542-B64F9933F7A8}" name="site" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{BA067983-0C25-7A45-B542-B64F9933F7A8}" name="site" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{1AC69149-64EF-6441-8851-05C55394873F}" name="dhcp_vrf"/>
     <tableColumn id="6" xr3:uid="{28B7873A-4A5B-AB43-A889-A94DEDDFEB56}" name="dhcp_address"/>
     <tableColumn id="7" xr3:uid="{6D6EDB65-10DD-0F41-8DF3-3E44B04E7296}" name="status"/>
@@ -2277,10 +2278,10 @@
       <c r="A1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D1" t="s">
@@ -2288,7 +2289,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <f>_xlfn.XLOOKUP(Table7[[#This Row],[template_name]],schema[template],schema[name])</f>
         <v>0</v>
       </c>
@@ -2377,20 +2378,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="8" t="str">
+      <c r="D2" s="7" t="str">
         <f>IF(ISBLANK(vrf[[#This Row],[name]]),"",_xlfn.XLOOKUP(vrf[[#This Row],[template_name]],schema[template],schema[name]))</f>
         <v/>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="7">
@@ -2448,28 +2439,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="str">
+      <c r="B2" s="7" t="str">
         <f>IF(ISBLANK(vrf_site_association[[#This Row],[vrf_name]]),"",_xlfn.XLOOKUP(vrf_site_association[[#This Row],[vrf_name]],vrf[name],vrf[template_name]))</f>
         <v/>
       </c>
-      <c r="C2" s="8" t="str">
+      <c r="C2" s="7" t="str">
         <f>IF(ISBLANK(vrf_site_association[[#This Row],[vrf_name]]),"",_xlfn.XLOOKUP(vrf_site_association[[#This Row],[vrf_name]],vrf[name],vrf[schema_name]))</f>
         <v/>
       </c>
@@ -2517,41 +2508,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="str">
+      <c r="B2" s="7" t="str">
         <f>IF(ISBLANK(vrf_site_switch_association[[#This Row],[vrf_name]]),"",_xlfn.XLOOKUP(vrf_site_switch_association[[#This Row],[vrf_name]],vrf[name],vrf[template_name]))</f>
         <v/>
       </c>
-      <c r="C2" s="8" t="str">
+      <c r="C2" s="7" t="str">
         <f>IF(ISBLANK(vrf_site_switch_association[[#This Row],[vrf_name]]),"",_xlfn.XLOOKUP(vrf_site_switch_association[[#This Row],[vrf_name]],vrf[name],vrf[schema_name]))</f>
         <v/>
       </c>
-      <c r="G2" s="8" t="str">
+      <c r="G2" s="7" t="str">
         <f>IF(ISBLANK(vrf_site_switch_association[[#This Row],[switch_1_serial_number]]),"",IF(ISBLANK(vrf_site_switch_association[[#This Row],[switch_2_serial_number]]),vrf_site_switch_association[[#This Row],[switch_1_serial_number]],vrf_site_switch_association[[#This Row],[switch_1_serial_number]]&amp;"~"&amp;vrf_site_switch_association[[#This Row],[switch_2_serial_number]]))</f>
         <v/>
       </c>
@@ -2666,15 +2657,15 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D2" s="8" t="str">
+      <c r="D2" s="7" t="str">
         <f>IF(ISBLANK(network[[#This Row],[vrf_name]]),"",_xlfn.XLOOKUP(network[[#This Row],[template_name]],schema[template],schema[name]))</f>
         <v/>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <f>_xlfn.XLOOKUP(network[[#This Row],[vrf_name]],vrf[name],vrf[template_name])</f>
         <v>0</v>
       </c>
-      <c r="I2" s="8" t="str">
+      <c r="I2" s="7" t="str">
         <f>_xlfn.XLOOKUP(network[[#This Row],[vrf_name]],vrf[name],vrf[schema_name])</f>
         <v/>
       </c>
@@ -2738,41 +2729,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="str">
+      <c r="B2" s="7" t="str">
         <f>IF(ISBLANK(network_site_association[[#This Row],[network_name]]),"",_xlfn.XLOOKUP(network_site_association[[#This Row],[network_name]],network[name],network[template_name]))</f>
         <v/>
       </c>
-      <c r="C2" s="8" t="str">
+      <c r="C2" s="7" t="str">
         <f>IF(ISBLANK(network_site_association[[#This Row],[network_name]]),"",_xlfn.XLOOKUP(network_site_association[[#This Row],[network_name]],network[name],network[schema_name]))</f>
         <v/>
       </c>
-      <c r="F2" s="8" t="str">
+      <c r="F2" s="7" t="str">
         <f>IF(ISBLANK(network_site_association[[#This Row],[network_name]]),"",_xlfn.XLOOKUP(network_site_association[[#This Row],[network_name]],network[name],network[vrf_name]))</f>
         <v/>
       </c>
@@ -2824,41 +2815,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="str">
+      <c r="B2" s="7" t="str">
         <f>IF(ISBLANK(network_site_association16[[#This Row],[network_name]]),"",_xlfn.XLOOKUP(network_site_association16[[#This Row],[network_name]],network[name],network[template_name]))</f>
         <v/>
       </c>
-      <c r="C2" s="8" t="str">
+      <c r="C2" s="7" t="str">
         <f>IF(ISBLANK(network_site_association16[[#This Row],[network_name]]),"",_xlfn.XLOOKUP(network_site_association16[[#This Row],[network_name]],network[name],network[schema_name]))</f>
         <v/>
       </c>
-      <c r="G2" s="8" t="str">
+      <c r="G2" s="7" t="str">
         <f>IF(ISBLANK(network_site_association16[[#This Row],[switch_1_serial_number]]),"",IF(ISBLANK(network_site_association16[[#This Row],[switch_2_serial_number]]),network_site_association16[[#This Row],[switch_1_serial_number]],network_site_association16[[#This Row],[switch_1_serial_number]]&amp;"~"&amp;network_site_association16[[#This Row],[switch_2_serial_number]]))</f>
         <v/>
       </c>
@@ -2893,7 +2884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FEB71F8-566C-9441-804A-C4150C34C987}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -2906,39 +2897,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14" t="str">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13" t="str">
         <f>IF(ISBLANK(network_site_association16[[#This Row],[network_name]]),"",_xlfn.XLOOKUP(network_site_association16[[#This Row],[network_name]],network[name],network[template_name]))</f>
         <v/>
       </c>
-      <c r="C2" s="14" t="str">
+      <c r="C2" s="13" t="str">
         <f>IF(ISBLANK(network_site_association16[[#This Row],[network_name]]),"",_xlfn.XLOOKUP(network_site_association16[[#This Row],[network_name]],network[name],network[schema_name]))</f>
         <v/>
       </c>
-      <c r="D2" s="13"/>
+      <c r="D2" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2970,8 +2961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD8639C-5D7A-4641-9C8D-4A8EC322A8E2}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScale="268" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="268" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2983,19 +2974,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3009,7 +3000,9 @@
       <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3072,10 +3065,10 @@
       <c r="H1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>44</v>
       </c>
       <c r="K1" t="s">
@@ -3083,17 +3076,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="H2" s="8" t="str">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="H2" s="7" t="str">
         <f>IF(site[[#This Row],[dcnm_fabric_type]] = "External","External","VxlanFabric")</f>
         <v>VxlanFabric</v>
       </c>
-      <c r="I2" s="11" cm="1">
+      <c r="I2" s="10" cm="1">
         <f t="array" ref="I2">infra_dcnm_config[multisite_loopback_range]</f>
         <v>0</v>
       </c>
-      <c r="J2" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -3181,24 +3173,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3296,11 +3285,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3336,16 +3324,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3378,7 +3366,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D934BC9-901E-2E4A-A53E-5A76FE795642}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView zoomScale="395" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -3407,13 +3395,6 @@
       <c r="E1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="5">

</xml_diff>